<commit_message>
Giving up for tonight, need to ask some questions
</commit_message>
<xml_diff>
--- a/Homework_1/ControlSignals.xlsx
+++ b/Homework_1/ControlSignals.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\_Second Year\Computer Architectures\assesment\MyMicroProccessor\InstructionSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\_Second Year\Computer Architectures\assesment\MyMicroProccessor\Homework_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12045"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Control Signals" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>Command</t>
   </si>
@@ -126,13 +126,28 @@
   </si>
   <si>
     <t>ØØØ0</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>0xAF1F</t>
+  </si>
+  <si>
+    <t>ØØ1Ø</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>ØØØ1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +169,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -428,15 +449,9 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -455,18 +470,60 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M16"/>
+  <dimension ref="B1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,48 +825,48 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -844,8 +901,8 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="18" t="s">
@@ -880,8 +937,8 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -916,8 +973,8 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -952,93 +1009,193 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="23"/>
+      <c r="D7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="21"/>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="25"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
+      <c r="B12" s="5"/>
+      <c r="C12" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -1052,9 +1209,9 @@
       <c r="M12" s="21"/>
     </row>
     <row r="13" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
+      <c r="B13" s="5"/>
+      <c r="C13" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -1067,59 +1224,27 @@
       <c r="L13" s="18"/>
       <c r="M13" s="19"/>
     </row>
-    <row r="14" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
-    </row>
-    <row r="15" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="2:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="9" t="s">
+    <row r="14" spans="2:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="27"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>